<commit_message>
Updated the order of Suppl files
</commit_message>
<xml_diff>
--- a/suppl_data/SupplData4 - statistic_AFTR-orthologs_Streptomyces.xlsx
+++ b/suppl_data/SupplData4 - statistic_AFTR-orthologs_Streptomyces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/_my/github/article-tta-codon/suppl_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECBFA79-B740-C34A-9EB5-20297288DCC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8F1B15-E41D-BA4E-A7E3-336199E02757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1960" windowWidth="38400" windowHeight="18040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="38400" windowHeight="18040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unique_AFTR-orthologs_Streptomy" sheetId="1" r:id="rId1"/>
@@ -3301,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12007,8 +12007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>